<commit_message>
28/11/22 - 12h24 - Debut MCD
</commit_message>
<xml_diff>
--- a/Exercices/90 - Fil Rouge/2. Conception/Dictionnaire des Données.xlsx
+++ b/Exercices/90 - Fil Rouge/2. Conception/Dictionnaire des Données.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\AFPA_CDA\Exercices\90 - Fil Rouge\2. Conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D9E802-09C3-4863-B223-375F656FA835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E29BA54-17EF-4935-8D9E-D3365E7ADBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="159">
   <si>
     <t>Commentaires</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Lien de la photo pour un href</t>
   </si>
   <si>
-    <t>TINYBLOB</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Produits</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>nomFournisseur</t>
   </si>
   <si>
-    <t>9 chiffres + (0 ou code international[+XXX]) + 4 séparateurs possibles</t>
-  </si>
-  <si>
     <t>idem</t>
   </si>
   <si>
@@ -498,6 +492,24 @@
   </si>
   <si>
     <t>Nbre de question pour le client:</t>
+  </si>
+  <si>
+    <t>peut être NULL?</t>
+  </si>
+  <si>
+    <t>9 chiffres + (0 ou code international[+XXX]) + 4 séparateurs possibles, peut être NULL?</t>
+  </si>
+  <si>
+    <t>VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>Coefficient par défaut en fonction de la catégorie</t>
+  </si>
+  <si>
+    <t>coefCategorie</t>
   </si>
 </sst>
 </file>
@@ -896,7 +908,7 @@
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1180,13 +1192,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
@@ -1378,6 +1390,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="25">
@@ -1714,13 +1738,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C73" sqref="C73"/>
+      <selection pane="bottomRight" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,7 +1764,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
@@ -1755,16 +1779,16 @@
         <v>0</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D2" s="33" t="s">
         <v>5</v>
@@ -1780,16 +1804,16 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="35"/>
       <c r="B3" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>95</v>
-      </c>
       <c r="E3" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="53"/>
@@ -1842,7 +1866,7 @@
         <v>21</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="54"/>
@@ -1859,7 +1883,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>26</v>
@@ -1888,13 +1912,13 @@
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="36"/>
       <c r="B9" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="D9" s="50" t="s">
         <v>73</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>74</v>
       </c>
       <c r="E9" s="51" t="s">
         <v>6</v>
@@ -1905,11 +1929,11 @@
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="15"/>
       <c r="C11" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>17</v>
@@ -1925,13 +1949,13 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>32</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>10</v>
@@ -1942,33 +1966,33 @@
     <row r="13" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" s="58"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="27" t="s">
         <v>6</v>
@@ -1981,13 +2005,13 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
       <c r="B16" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="24" t="s">
         <v>6</v>
@@ -1998,16 +2022,16 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="28"/>
       <c r="B17" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="21" t="s">
-        <v>45</v>
-      </c>
       <c r="E17" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="61"/>
@@ -2017,10 +2041,10 @@
       <c r="B18" s="23"/>
       <c r="C18" s="23"/>
       <c r="D18" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="60"/>
@@ -2028,13 +2052,13 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
       <c r="B19" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" s="22" t="s">
         <v>6</v>
@@ -2047,13 +2071,13 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="28"/>
       <c r="B20" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="24" t="s">
         <v>6</v>
@@ -2066,78 +2090,82 @@
     <row r="21" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="29"/>
       <c r="B21" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="31" t="s">
         <v>22</v>
       </c>
       <c r="F21" s="30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G21" s="62"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" s="40"/>
       <c r="C23" s="40" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" s="41" t="s">
         <v>6</v>
       </c>
       <c r="F23" s="40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G23" s="63"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="42"/>
       <c r="B24" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="44" t="s">
-        <v>62</v>
-      </c>
       <c r="D24" s="44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="44"/>
-      <c r="G24" s="64"/>
+      <c r="F24" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="G24" s="64" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="42"/>
       <c r="B25" s="37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="F25" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="37" t="s">
-        <v>64</v>
-      </c>
       <c r="G25" s="65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2145,62 +2173,62 @@
       <c r="B26" s="48"/>
       <c r="C26" s="48"/>
       <c r="D26" s="44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" s="45" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G26" s="64"/>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="42"/>
       <c r="B27" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="37"/>
       <c r="D27" s="37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F27" s="37" t="s">
-        <v>79</v>
+        <v>154</v>
       </c>
       <c r="G27" s="65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="43"/>
       <c r="B28" s="49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="49"/>
       <c r="D28" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="47" t="s">
-        <v>70</v>
-      </c>
       <c r="F28" s="46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G28" s="66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" s="68"/>
       <c r="C30" s="68" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D30" s="68" t="s">
         <v>16</v>
@@ -2216,13 +2244,13 @@
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="71"/>
       <c r="B31" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="72" t="s">
+      <c r="D31" s="72" t="s">
         <v>77</v>
-      </c>
-      <c r="D31" s="72" t="s">
-        <v>78</v>
       </c>
       <c r="E31" s="73" t="s">
         <v>10</v>
@@ -2233,14 +2261,14 @@
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="77" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B33" s="78"/>
       <c r="C33" s="78" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D33" s="78" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E33" s="79" t="s">
         <v>6</v>
@@ -2253,35 +2281,35 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="81"/>
       <c r="B34" s="87" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C34" s="87" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D34" s="87" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E34" s="88" t="s">
         <v>6</v>
       </c>
       <c r="F34" s="87" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G34" s="89"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="81"/>
       <c r="B35" s="75" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C35" s="75" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="75" t="s">
-        <v>90</v>
-      </c>
       <c r="E35" s="76" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F35" s="75"/>
       <c r="G35" s="82"/>
@@ -2290,10 +2318,10 @@
       <c r="A36" s="81"/>
       <c r="B36" s="87"/>
       <c r="C36" s="87" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D36" s="87" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E36" s="88" t="s">
         <v>6</v>
@@ -2307,10 +2335,10 @@
       <c r="A37" s="81"/>
       <c r="B37" s="75"/>
       <c r="C37" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="75" t="s">
         <v>97</v>
-      </c>
-      <c r="D37" s="75" t="s">
-        <v>99</v>
       </c>
       <c r="E37" s="76" t="s">
         <v>6</v>
@@ -2324,10 +2352,10 @@
       <c r="A38" s="136"/>
       <c r="B38" s="137"/>
       <c r="C38" s="137" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="137" t="s">
         <v>98</v>
-      </c>
-      <c r="D38" s="137" t="s">
-        <v>100</v>
       </c>
       <c r="E38" s="138" t="s">
         <v>6</v>
@@ -2341,10 +2369,10 @@
       <c r="A39" s="83"/>
       <c r="B39" s="84"/>
       <c r="C39" s="84" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D39" s="84" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E39" s="85" t="s">
         <v>6</v>
@@ -2357,12 +2385,12 @@
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="90" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B41" s="91"/>
       <c r="C41" s="91"/>
       <c r="D41" s="91" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E41" s="92" t="s">
         <v>6</v>
@@ -2372,378 +2400,395 @@
       </c>
       <c r="G41" s="93"/>
     </row>
-    <row r="42" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="94"/>
-      <c r="B42" s="95" t="s">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="164"/>
+      <c r="B42" s="162" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="162" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="95" t="s">
+      <c r="D42" s="162" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" s="163" t="s">
+        <v>53</v>
+      </c>
+      <c r="F42" s="162"/>
+      <c r="G42" s="165"/>
+    </row>
+    <row r="43" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="94"/>
+      <c r="B43" s="95" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43" s="95" t="s">
+        <v>157</v>
+      </c>
+      <c r="D43" s="95" t="s">
+        <v>158</v>
+      </c>
+      <c r="E43" s="96" t="s">
+        <v>22</v>
+      </c>
+      <c r="F43" s="95"/>
+      <c r="G43" s="97"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="100" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" s="101" t="s">
         <v>103</v>
       </c>
-      <c r="D42" s="95" t="s">
+      <c r="C45" s="101" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="101" t="s">
         <v>104</v>
       </c>
-      <c r="E42" s="96" t="s">
-        <v>54</v>
-      </c>
-      <c r="F42" s="95"/>
-      <c r="G42" s="97"/>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="100" t="s">
-        <v>116</v>
-      </c>
-      <c r="B44" s="101" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="101" t="s">
-        <v>111</v>
-      </c>
-      <c r="D44" s="101" t="s">
-        <v>106</v>
-      </c>
-      <c r="E44" s="102" t="s">
+      <c r="E45" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="101" t="s">
+      <c r="F45" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="G44" s="103"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="104"/>
-      <c r="B45" s="110" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" s="110" t="s">
-        <v>112</v>
-      </c>
-      <c r="D45" s="110" t="s">
-        <v>107</v>
-      </c>
-      <c r="E45" s="111" t="s">
-        <v>10</v>
-      </c>
-      <c r="F45" s="110"/>
-      <c r="G45" s="112"/>
+      <c r="G45" s="103"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="104"/>
-      <c r="B46" s="98" t="s">
+      <c r="B46" s="110" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="110" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="110" t="s">
         <v>105</v>
       </c>
-      <c r="C46" s="98" t="s">
-        <v>113</v>
-      </c>
-      <c r="D46" s="98" t="s">
-        <v>108</v>
-      </c>
-      <c r="E46" s="99" t="s">
+      <c r="E46" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="F46" s="98" t="s">
-        <v>87</v>
-      </c>
-      <c r="G46" s="105"/>
+      <c r="F46" s="110"/>
+      <c r="G46" s="112"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="104"/>
-      <c r="B47" s="110" t="s">
-        <v>105</v>
-      </c>
-      <c r="C47" s="110" t="s">
-        <v>114</v>
-      </c>
-      <c r="D47" s="110" t="s">
-        <v>109</v>
-      </c>
-      <c r="E47" s="111" t="s">
+      <c r="B47" s="98" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="D47" s="98" t="s">
+        <v>106</v>
+      </c>
+      <c r="E47" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="F47" s="110"/>
-      <c r="G47" s="112"/>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="106"/>
-      <c r="B48" s="107"/>
-      <c r="C48" s="107"/>
-      <c r="D48" s="107" t="s">
-        <v>36</v>
-      </c>
-      <c r="E48" s="108" t="s">
+      <c r="F47" s="98" t="s">
+        <v>85</v>
+      </c>
+      <c r="G47" s="105"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="104"/>
+      <c r="B48" s="110" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="110" t="s">
+        <v>112</v>
+      </c>
+      <c r="D48" s="110" t="s">
+        <v>107</v>
+      </c>
+      <c r="E48" s="111" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="110"/>
+      <c r="G48" s="112"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="106"/>
+      <c r="B49" s="107"/>
+      <c r="C49" s="107"/>
+      <c r="D49" s="107" t="s">
+        <v>35</v>
+      </c>
+      <c r="E49" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="F48" s="107" t="s">
+      <c r="F49" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="G48" s="109" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="113" t="s">
+      <c r="G49" s="109" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="113" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" s="114"/>
+      <c r="C51" s="114"/>
+      <c r="D51" s="114" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="114"/>
-      <c r="C50" s="114"/>
-      <c r="D50" s="114" t="s">
+      <c r="E51" s="115" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="114" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="116"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="142"/>
+      <c r="B52" s="140" t="s">
         <v>117</v>
       </c>
-      <c r="E50" s="115" t="s">
+      <c r="C52" s="140" t="s">
+        <v>118</v>
+      </c>
+      <c r="D52" s="140" t="s">
+        <v>116</v>
+      </c>
+      <c r="E52" s="141" t="s">
+        <v>22</v>
+      </c>
+      <c r="F52" s="140"/>
+      <c r="G52" s="143"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="117"/>
+      <c r="B53" s="118"/>
+      <c r="C53" s="118" t="s">
+        <v>141</v>
+      </c>
+      <c r="D53" s="118" t="s">
+        <v>142</v>
+      </c>
+      <c r="E53" s="119" t="s">
+        <v>89</v>
+      </c>
+      <c r="F53" s="118"/>
+      <c r="G53" s="144"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="120" t="s">
+        <v>119</v>
+      </c>
+      <c r="B55" s="121"/>
+      <c r="C55" s="121"/>
+      <c r="D55" s="121" t="s">
+        <v>120</v>
+      </c>
+      <c r="E55" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="F50" s="114" t="s">
+      <c r="F55" s="121"/>
+      <c r="G55" s="123"/>
+    </row>
+    <row r="56" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="124"/>
+      <c r="B56" s="125" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="125" t="s">
+        <v>126</v>
+      </c>
+      <c r="D56" s="125" t="s">
+        <v>121</v>
+      </c>
+      <c r="E56" s="126" t="s">
+        <v>53</v>
+      </c>
+      <c r="F56" s="125"/>
+      <c r="G56" s="127"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="128" t="s">
+        <v>123</v>
+      </c>
+      <c r="B58" s="129"/>
+      <c r="C58" s="129"/>
+      <c r="D58" s="129" t="s">
+        <v>124</v>
+      </c>
+      <c r="E58" s="130" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" s="129" t="s">
         <v>7</v>
       </c>
-      <c r="G50" s="116"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="142"/>
-      <c r="B51" s="140" t="s">
-        <v>119</v>
-      </c>
-      <c r="C51" s="140" t="s">
-        <v>120</v>
-      </c>
-      <c r="D51" s="140" t="s">
-        <v>118</v>
-      </c>
-      <c r="E51" s="141" t="s">
-        <v>22</v>
-      </c>
-      <c r="F51" s="140"/>
-      <c r="G51" s="143"/>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="117"/>
-      <c r="B52" s="118"/>
-      <c r="C52" s="118" t="s">
-        <v>143</v>
-      </c>
-      <c r="D52" s="118" t="s">
-        <v>144</v>
-      </c>
-      <c r="E52" s="119" t="s">
-        <v>91</v>
-      </c>
-      <c r="F52" s="118"/>
-      <c r="G52" s="144"/>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="120" t="s">
-        <v>121</v>
-      </c>
-      <c r="B54" s="121"/>
-      <c r="C54" s="121"/>
-      <c r="D54" s="121" t="s">
-        <v>122</v>
-      </c>
-      <c r="E54" s="122" t="s">
-        <v>6</v>
-      </c>
-      <c r="F54" s="121"/>
-      <c r="G54" s="123"/>
-    </row>
-    <row r="55" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="124"/>
-      <c r="B55" s="125" t="s">
-        <v>124</v>
-      </c>
-      <c r="C55" s="125" t="s">
+      <c r="G58" s="131"/>
+    </row>
+    <row r="59" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="132"/>
+      <c r="B59" s="133" t="s">
+        <v>129</v>
+      </c>
+      <c r="C59" s="133" t="s">
         <v>128</v>
       </c>
-      <c r="D55" s="125" t="s">
-        <v>123</v>
-      </c>
-      <c r="E55" s="126" t="s">
-        <v>54</v>
-      </c>
-      <c r="F55" s="125"/>
-      <c r="G55" s="127"/>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="128" t="s">
+      <c r="D59" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="B57" s="129"/>
-      <c r="C57" s="129"/>
-      <c r="D57" s="129" t="s">
-        <v>126</v>
-      </c>
-      <c r="E57" s="130" t="s">
-        <v>6</v>
-      </c>
-      <c r="F57" s="129" t="s">
-        <v>7</v>
-      </c>
-      <c r="G57" s="131"/>
-    </row>
-    <row r="58" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="132"/>
-      <c r="B58" s="133" t="s">
+      <c r="E59" s="134" t="s">
+        <v>53</v>
+      </c>
+      <c r="F59" s="133" t="s">
+        <v>127</v>
+      </c>
+      <c r="G59" s="135"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="150" t="s">
         <v>131</v>
       </c>
-      <c r="C58" s="133" t="s">
-        <v>130</v>
-      </c>
-      <c r="D58" s="133" t="s">
-        <v>127</v>
-      </c>
-      <c r="E58" s="134" t="s">
-        <v>54</v>
-      </c>
-      <c r="F58" s="133" t="s">
+      <c r="B61" s="151" t="s">
         <v>129</v>
       </c>
-      <c r="G58" s="135"/>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="150" t="s">
+      <c r="C61" s="151" t="s">
+        <v>132</v>
+      </c>
+      <c r="D61" s="151" t="s">
         <v>133</v>
       </c>
-      <c r="B60" s="151" t="s">
-        <v>131</v>
-      </c>
-      <c r="C60" s="151" t="s">
+      <c r="E61" s="152" t="s">
+        <v>89</v>
+      </c>
+      <c r="F61" s="151" t="s">
         <v>134</v>
       </c>
-      <c r="D60" s="151" t="s">
-        <v>135</v>
-      </c>
-      <c r="E60" s="152" t="s">
-        <v>91</v>
-      </c>
-      <c r="F60" s="151" t="s">
-        <v>136</v>
-      </c>
-      <c r="G60" s="153"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="154"/>
-      <c r="B61" s="147" t="s">
-        <v>124</v>
-      </c>
-      <c r="C61" s="148" t="s">
-        <v>138</v>
-      </c>
-      <c r="D61" s="148" t="s">
-        <v>140</v>
-      </c>
-      <c r="E61" s="149" t="s">
-        <v>137</v>
-      </c>
-      <c r="F61" s="148" t="s">
-        <v>142</v>
-      </c>
-      <c r="G61" s="155"/>
+      <c r="G61" s="153"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="154"/>
-      <c r="B62" s="145"/>
-      <c r="C62" s="145" t="s">
-        <v>139</v>
-      </c>
-      <c r="D62" s="145" t="s">
-        <v>141</v>
-      </c>
-      <c r="E62" s="146" t="s">
-        <v>91</v>
-      </c>
-      <c r="F62" s="145" t="s">
-        <v>80</v>
-      </c>
-      <c r="G62" s="156"/>
+      <c r="B62" s="147" t="s">
+        <v>122</v>
+      </c>
+      <c r="C62" s="148" t="s">
+        <v>136</v>
+      </c>
+      <c r="D62" s="148" t="s">
+        <v>138</v>
+      </c>
+      <c r="E62" s="149" t="s">
+        <v>135</v>
+      </c>
+      <c r="F62" s="148" t="s">
+        <v>140</v>
+      </c>
+      <c r="G62" s="155"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="154"/>
-      <c r="B63" s="148" t="s">
-        <v>145</v>
-      </c>
-      <c r="C63" s="148" t="s">
-        <v>146</v>
-      </c>
-      <c r="D63" s="148" t="s">
-        <v>147</v>
-      </c>
-      <c r="E63" s="149" t="s">
-        <v>6</v>
-      </c>
-      <c r="F63" s="148" t="s">
-        <v>148</v>
-      </c>
-      <c r="G63" s="155"/>
+      <c r="B63" s="145"/>
+      <c r="C63" s="145" t="s">
+        <v>137</v>
+      </c>
+      <c r="D63" s="145" t="s">
+        <v>139</v>
+      </c>
+      <c r="E63" s="146" t="s">
+        <v>89</v>
+      </c>
+      <c r="F63" s="145" t="s">
+        <v>78</v>
+      </c>
+      <c r="G63" s="156"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="154"/>
-      <c r="B64" s="145" t="s">
+      <c r="B64" s="148" t="s">
+        <v>143</v>
+      </c>
+      <c r="C64" s="148" t="s">
+        <v>144</v>
+      </c>
+      <c r="D64" s="148" t="s">
+        <v>145</v>
+      </c>
+      <c r="E64" s="149" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" s="148" t="s">
+        <v>146</v>
+      </c>
+      <c r="G64" s="155"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="154"/>
+      <c r="B65" s="145" t="s">
+        <v>147</v>
+      </c>
+      <c r="C65" s="145" t="s">
+        <v>148</v>
+      </c>
+      <c r="D65" s="145" t="s">
+        <v>150</v>
+      </c>
+      <c r="E65" s="146" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" s="145" t="s">
+        <v>78</v>
+      </c>
+      <c r="G65" s="156"/>
+    </row>
+    <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="157"/>
+      <c r="B66" s="158"/>
+      <c r="C66" s="158" t="s">
         <v>149</v>
       </c>
-      <c r="C64" s="145" t="s">
-        <v>150</v>
-      </c>
-      <c r="D64" s="145" t="s">
+      <c r="D66" s="158" t="s">
+        <v>151</v>
+      </c>
+      <c r="E66" s="159" t="s">
+        <v>89</v>
+      </c>
+      <c r="F66" s="158" t="s">
+        <v>78</v>
+      </c>
+      <c r="G66" s="160"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F68" s="161" t="s">
         <v>152</v>
       </c>
-      <c r="E64" s="146" t="s">
-        <v>6</v>
-      </c>
-      <c r="F64" s="145" t="s">
-        <v>80</v>
-      </c>
-      <c r="G64" s="156"/>
-    </row>
-    <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="157"/>
-      <c r="B65" s="158"/>
-      <c r="C65" s="158" t="s">
-        <v>151</v>
-      </c>
-      <c r="D65" s="158" t="s">
-        <v>153</v>
-      </c>
-      <c r="E65" s="159" t="s">
-        <v>91</v>
-      </c>
-      <c r="F65" s="158" t="s">
-        <v>80</v>
-      </c>
-      <c r="G65" s="160"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F67" s="161" t="s">
-        <v>154</v>
-      </c>
-      <c r="G67" s="7">
-        <f>COUNTA(G2:G65)</f>
-        <v>4</v>
+      <c r="G68" s="7">
+        <f>COUNTA(G2:G66)</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A60:A65"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A61:A66"/>
     <mergeCell ref="A23:A28"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A33:A39"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A51:A53"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A15:A21"/>
   </mergeCells>
-  <conditionalFormatting sqref="G1:G51 G53:G1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <conditionalFormatting sqref="G54:G1048576 G1:G52">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Oui"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G67">
+  <conditionalFormatting sqref="G68">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
28/11/22 - 15h26 - Correct du DdD & MCD V2
</commit_message>
<xml_diff>
--- a/Exercices/90 - Fil Rouge/2. Conception/Dictionnaire des Données.xlsx
+++ b/Exercices/90 - Fil Rouge/2. Conception/Dictionnaire des Données.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\AFPA_CDA\Exercices\90 - Fil Rouge\2. Conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E29BA54-17EF-4935-8D9E-D3365E7ADBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B784B5A-ABC1-4F58-A6AC-A7034F526B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1473,6 +1473,128 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3000375</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0547825F-7BFD-9379-36CD-C0C9723203A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1657349" y="14878050"/>
+          <a:ext cx="9582151" cy="1905000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Erreurs:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>- Confusion entre le</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> libellé court et la référence du produit =&gt; à entrainé en plus le choix d'un format trop court pour la description;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Pas présent dans correction ni version perso mais, après réflexion, numClient devrait être UNIQUE;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Oublis des info de réglement dans CategoriesClients;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- dateValiditeTVA mis au mauvais endroit</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- J'ai pensé à mettre les adresses dans leurs propre table mais n'ai pas séparé les villes et codes postaux (noté comme question à poser au client) ni les pays (n'y ai pas pensé du tout);</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- J'ai pensé aux utilisateurs mais pas à leur appliquer un rôle;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>- Pas pensé à la possibilité que la référence du produit pour l'entreprise pourrait être différente de celle du fournisseur...</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1741,10 +1863,10 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I43" sqref="I43"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2795,5 +2917,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
28/11/22 - 17h53 - Script Gest Droits FilRouge
</commit_message>
<xml_diff>
--- a/Exercices/90 - Fil Rouge/2. Conception/Dictionnaire des Données.xlsx
+++ b/Exercices/90 - Fil Rouge/2. Conception/Dictionnaire des Données.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\AFPA_CDA\Exercices\90 - Fil Rouge\2. Conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B784B5A-ABC1-4F58-A6AC-A7034F526B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FF9FE7-21C9-48A8-9B27-531E4A9187C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1431,17 +1431,7 @@
     <cellStyle name="Accent6" xfId="21" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1480,13 +1470,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
+      <xdr:colOff>19051</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>3000375</xdr:colOff>
+      <xdr:colOff>3000376</xdr:colOff>
       <xdr:row>78</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -1503,8 +1493,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1657349" y="14878050"/>
-          <a:ext cx="9582151" cy="1905000"/>
+          <a:off x="1562101" y="14878050"/>
+          <a:ext cx="9677400" cy="1905000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1587,6 +1577,15 @@
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
             <a:t>- Pas pensé à la possibilité que la référence du produit pour l'entreprise pourrait être différente de celle du fournisseur...</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>Dans correction, manque entrée pour les états possible de la commande...</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>

</xml_diff>

<commit_message>
28/11/22 - 19h08 - Debut JdD Fil Rouge
</commit_message>
<xml_diff>
--- a/Exercices/90 - Fil Rouge/2. Conception/Dictionnaire des Données.xlsx
+++ b/Exercices/90 - Fil Rouge/2. Conception/Dictionnaire des Données.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\AFPA_CDA\Exercices\90 - Fil Rouge\2. Conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FF9FE7-21C9-48A8-9B27-531E4A9187C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1AE332-AB41-4C9C-AB54-FEFBA6A31118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -949,21 +949,12 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -982,63 +973,36 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="7" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="14" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1108,9 +1072,6 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="9" xfId="14" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="2" xfId="19" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="3" xfId="19" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1120,9 +1081,6 @@
     <xf numFmtId="0" fontId="1" fillId="20" borderId="4" xfId="19" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="7" xfId="19" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="18" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1138,9 +1096,6 @@
     <xf numFmtId="0" fontId="1" fillId="24" borderId="1" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="2" xfId="23" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="3" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1150,15 +1105,9 @@
     <xf numFmtId="0" fontId="1" fillId="24" borderId="4" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="5" xfId="23" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="6" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="7" xfId="23" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="8" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1177,9 +1126,6 @@
     <xf numFmtId="0" fontId="1" fillId="23" borderId="6" xfId="22" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1189,9 +1135,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1207,9 +1150,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1219,15 +1159,9 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1246,9 +1180,6 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1258,18 +1189,12 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="3" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1279,9 +1204,6 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="7" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="8" xfId="16" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1291,9 +1213,6 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="16" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="17" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="3" xfId="17" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1303,9 +1222,6 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="4" xfId="17" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="7" xfId="17" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="8" xfId="20" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1315,9 +1231,6 @@
     <xf numFmtId="0" fontId="1" fillId="21" borderId="9" xfId="20" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="12" xfId="23" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="10" xfId="22" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1332,9 +1245,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1355,9 +1265,6 @@
     <xf numFmtId="0" fontId="1" fillId="25" borderId="1" xfId="24" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="2" xfId="21" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="3" xfId="21" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1367,16 +1274,10 @@
     <xf numFmtId="0" fontId="2" fillId="22" borderId="4" xfId="21" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="5" xfId="21" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="6" xfId="24" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="6" xfId="21" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="7" xfId="21" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="8" xfId="24" applyBorder="1" applyAlignment="1">
@@ -1397,10 +1298,109 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="7" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="7" xfId="17" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="2" xfId="21" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="5" xfId="21" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="7" xfId="21" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="7" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="2" xfId="19" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="7" xfId="19" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="2" xfId="23" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="5" xfId="23" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="12" xfId="23" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="7" xfId="23" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1862,10 +1862,10 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1904,26 +1904,26 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="157" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="52"/>
+      <c r="G2" s="40"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
+      <c r="A3" s="158"/>
       <c r="B3" s="10" t="s">
         <v>91</v>
       </c>
@@ -1937,10 +1937,10 @@
         <v>90</v>
       </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="53"/>
+      <c r="G3" s="41"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="158"/>
       <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
@@ -1954,10 +1954,10 @@
         <v>10</v>
       </c>
       <c r="F4" s="8"/>
-      <c r="G4" s="54"/>
+      <c r="G4" s="42"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="158"/>
       <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
@@ -1973,10 +1973,10 @@
       <c r="F5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="53"/>
+      <c r="G5" s="41"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
+      <c r="A6" s="158"/>
       <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
@@ -1990,10 +1990,10 @@
         <v>135</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="54"/>
+      <c r="G6" s="42"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="158"/>
       <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
@@ -2009,10 +2009,10 @@
       <c r="F7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="53"/>
+      <c r="G7" s="41"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="158"/>
       <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
@@ -2028,47 +2028,47 @@
       <c r="F8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="54"/>
+      <c r="G8" s="42"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
-      <c r="B9" s="50" t="s">
+      <c r="A9" s="159"/>
+      <c r="B9" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="50"/>
-      <c r="G9" s="55"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="43"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="160" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="56"/>
+      <c r="G11" s="44"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+      <c r="A12" s="161"/>
       <c r="B12" s="12" t="s">
         <v>28</v>
       </c>
@@ -2082,806 +2082,806 @@
         <v>10</v>
       </c>
       <c r="F12" s="12"/>
-      <c r="G12" s="57"/>
+      <c r="G12" s="45"/>
     </row>
     <row r="13" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19" t="s">
+      <c r="A13" s="162"/>
+      <c r="B13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="58"/>
+      <c r="G13" s="46"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="163" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="59"/>
+      <c r="G15" s="47"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="23" t="s">
+      <c r="A16" s="164"/>
+      <c r="B16" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="60"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="48"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="21" t="s">
+      <c r="A17" s="164"/>
+      <c r="B17" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="61"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="49"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23" t="s">
+      <c r="A18" s="164"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="60"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="48"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="164"/>
+      <c r="B19" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="61"/>
+      <c r="G19" s="49"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="164"/>
+      <c r="B20" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="60"/>
+      <c r="G20" s="48"/>
     </row>
     <row r="21" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="29"/>
-      <c r="B21" s="30" t="s">
+      <c r="A21" s="165"/>
+      <c r="B21" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="F21" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="62"/>
+      <c r="G21" s="50"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="139" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40" t="s">
+      <c r="B23" s="30"/>
+      <c r="C23" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="G23" s="63"/>
+      <c r="G23" s="51"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
-      <c r="B24" s="44" t="s">
+      <c r="A24" s="140"/>
+      <c r="B24" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="45" t="s">
+      <c r="E24" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="F24" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="G24" s="64" t="s">
+      <c r="G24" s="52" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
-      <c r="B25" s="37" t="s">
+      <c r="A25" s="140"/>
+      <c r="B25" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="F25" s="37" t="s">
+      <c r="F25" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="G25" s="65" t="s">
+      <c r="G25" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="44" t="s">
+      <c r="A26" s="140"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="45" t="s">
+      <c r="E26" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="44" t="s">
+      <c r="F26" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="64"/>
+      <c r="G26" s="52"/>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="37" t="s">
+      <c r="A27" s="140"/>
+      <c r="B27" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37" t="s">
+      <c r="C27" s="28"/>
+      <c r="D27" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="F27" s="37" t="s">
+      <c r="F27" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="G27" s="65" t="s">
+      <c r="G27" s="53" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="43"/>
-      <c r="B28" s="49" t="s">
+      <c r="A28" s="141"/>
+      <c r="B28" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="46" t="s">
+      <c r="C28" s="37"/>
+      <c r="D28" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="47" t="s">
+      <c r="E28" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="46" t="s">
+      <c r="F28" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="G28" s="66" t="s">
+      <c r="G28" s="54" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="67" t="s">
+      <c r="A30" s="142" t="s">
         <v>74</v>
       </c>
-      <c r="B30" s="68"/>
-      <c r="C30" s="68" t="s">
+      <c r="B30" s="55"/>
+      <c r="C30" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="D30" s="68" t="s">
+      <c r="D30" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="69" t="s">
+      <c r="E30" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="68" t="s">
+      <c r="F30" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="G30" s="70"/>
+      <c r="G30" s="57"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="71"/>
-      <c r="B31" s="72" t="s">
+      <c r="A31" s="143"/>
+      <c r="B31" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="72" t="s">
+      <c r="C31" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="72" t="s">
+      <c r="D31" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="73" t="s">
+      <c r="E31" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="72"/>
-      <c r="G31" s="74"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="60"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="77" t="s">
+      <c r="A33" s="144" t="s">
         <v>79</v>
       </c>
-      <c r="B33" s="78"/>
-      <c r="C33" s="78" t="s">
+      <c r="B33" s="63"/>
+      <c r="C33" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="78" t="s">
+      <c r="D33" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="79" t="s">
+      <c r="E33" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="78" t="s">
+      <c r="F33" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="G33" s="80"/>
+      <c r="G33" s="65"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="81"/>
-      <c r="B34" s="87" t="s">
+      <c r="A34" s="145"/>
+      <c r="B34" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="87" t="s">
+      <c r="C34" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="87" t="s">
+      <c r="D34" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="E34" s="88" t="s">
+      <c r="E34" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="87" t="s">
+      <c r="F34" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="G34" s="89"/>
+      <c r="G34" s="72"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="81"/>
-      <c r="B35" s="75" t="s">
+      <c r="A35" s="145"/>
+      <c r="B35" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="75" t="s">
+      <c r="C35" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="D35" s="75" t="s">
+      <c r="D35" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="E35" s="76" t="s">
+      <c r="E35" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="F35" s="75"/>
-      <c r="G35" s="82"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="66"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="81"/>
-      <c r="B36" s="87"/>
-      <c r="C36" s="87" t="s">
+      <c r="A36" s="145"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="D36" s="87" t="s">
+      <c r="D36" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="88" t="s">
+      <c r="E36" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="F36" s="87" t="s">
+      <c r="F36" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="G36" s="89"/>
+      <c r="G36" s="72"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="81"/>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75" t="s">
+      <c r="A37" s="145"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="75" t="s">
+      <c r="D37" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="E37" s="76" t="s">
+      <c r="E37" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="F37" s="75" t="s">
+      <c r="F37" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="82"/>
+      <c r="G37" s="66"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="136"/>
-      <c r="B38" s="137"/>
-      <c r="C38" s="137" t="s">
+      <c r="A38" s="146"/>
+      <c r="B38" s="108"/>
+      <c r="C38" s="108" t="s">
         <v>96</v>
       </c>
-      <c r="D38" s="137" t="s">
+      <c r="D38" s="108" t="s">
         <v>98</v>
       </c>
-      <c r="E38" s="138" t="s">
+      <c r="E38" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="F38" s="137" t="s">
+      <c r="F38" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="G38" s="139"/>
+      <c r="G38" s="110"/>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="83"/>
-      <c r="B39" s="84"/>
-      <c r="C39" s="84" t="s">
+      <c r="A39" s="147"/>
+      <c r="B39" s="67"/>
+      <c r="C39" s="67" t="s">
         <v>130</v>
       </c>
-      <c r="D39" s="84" t="s">
+      <c r="D39" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="E39" s="85" t="s">
+      <c r="E39" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="84" t="s">
+      <c r="F39" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="G39" s="86"/>
+      <c r="G39" s="69"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="90" t="s">
+      <c r="A41" s="148" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="91"/>
-      <c r="C41" s="91"/>
-      <c r="D41" s="91" t="s">
+      <c r="B41" s="73"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="92" t="s">
+      <c r="E41" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="F41" s="91" t="s">
+      <c r="F41" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="G41" s="93"/>
+      <c r="G41" s="75"/>
     </row>
     <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="164"/>
-      <c r="B42" s="162" t="s">
+      <c r="A42" s="149"/>
+      <c r="B42" s="129" t="s">
         <v>99</v>
       </c>
-      <c r="C42" s="162" t="s">
+      <c r="C42" s="129" t="s">
         <v>101</v>
       </c>
-      <c r="D42" s="162" t="s">
+      <c r="D42" s="129" t="s">
         <v>102</v>
       </c>
-      <c r="E42" s="163" t="s">
+      <c r="E42" s="130" t="s">
         <v>53</v>
       </c>
-      <c r="F42" s="162"/>
-      <c r="G42" s="165"/>
+      <c r="F42" s="129"/>
+      <c r="G42" s="131"/>
     </row>
     <row r="43" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="94"/>
-      <c r="B43" s="95" t="s">
+      <c r="A43" s="150"/>
+      <c r="B43" s="76" t="s">
         <v>156</v>
       </c>
-      <c r="C43" s="95" t="s">
+      <c r="C43" s="76" t="s">
         <v>157</v>
       </c>
-      <c r="D43" s="95" t="s">
+      <c r="D43" s="76" t="s">
         <v>158</v>
       </c>
-      <c r="E43" s="96" t="s">
+      <c r="E43" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="F43" s="95"/>
-      <c r="G43" s="97"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="78"/>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="100" t="s">
+      <c r="A45" s="151" t="s">
         <v>114</v>
       </c>
-      <c r="B45" s="101" t="s">
+      <c r="B45" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="C45" s="101" t="s">
+      <c r="C45" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="D45" s="101" t="s">
+      <c r="D45" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="E45" s="102" t="s">
+      <c r="E45" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="F45" s="101" t="s">
+      <c r="F45" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="G45" s="103"/>
+      <c r="G45" s="83"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="104"/>
-      <c r="B46" s="110" t="s">
+      <c r="A46" s="152"/>
+      <c r="B46" s="88" t="s">
         <v>103</v>
       </c>
-      <c r="C46" s="110" t="s">
+      <c r="C46" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="D46" s="110" t="s">
+      <c r="D46" s="88" t="s">
         <v>105</v>
       </c>
-      <c r="E46" s="111" t="s">
+      <c r="E46" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="F46" s="110"/>
-      <c r="G46" s="112"/>
+      <c r="F46" s="88"/>
+      <c r="G46" s="90"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="104"/>
-      <c r="B47" s="98" t="s">
+      <c r="A47" s="152"/>
+      <c r="B47" s="79" t="s">
         <v>103</v>
       </c>
-      <c r="C47" s="98" t="s">
+      <c r="C47" s="79" t="s">
         <v>111</v>
       </c>
-      <c r="D47" s="98" t="s">
+      <c r="D47" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="E47" s="99" t="s">
+      <c r="E47" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="F47" s="98" t="s">
+      <c r="F47" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="G47" s="105"/>
+      <c r="G47" s="84"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="104"/>
-      <c r="B48" s="110" t="s">
+      <c r="A48" s="152"/>
+      <c r="B48" s="88" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="110" t="s">
+      <c r="C48" s="88" t="s">
         <v>112</v>
       </c>
-      <c r="D48" s="110" t="s">
+      <c r="D48" s="88" t="s">
         <v>107</v>
       </c>
-      <c r="E48" s="111" t="s">
+      <c r="E48" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="F48" s="110"/>
-      <c r="G48" s="112"/>
+      <c r="F48" s="88"/>
+      <c r="G48" s="90"/>
     </row>
     <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="106"/>
-      <c r="B49" s="107"/>
-      <c r="C49" s="107"/>
-      <c r="D49" s="107" t="s">
+      <c r="A49" s="153"/>
+      <c r="B49" s="85"/>
+      <c r="C49" s="85"/>
+      <c r="D49" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="E49" s="108" t="s">
+      <c r="E49" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="F49" s="107" t="s">
+      <c r="F49" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="G49" s="109" t="s">
+      <c r="G49" s="87" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="113" t="s">
+      <c r="A51" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="B51" s="114"/>
-      <c r="C51" s="114"/>
-      <c r="D51" s="114" t="s">
+      <c r="B51" s="91"/>
+      <c r="C51" s="91"/>
+      <c r="D51" s="91" t="s">
         <v>115</v>
       </c>
-      <c r="E51" s="115" t="s">
+      <c r="E51" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="F51" s="114" t="s">
+      <c r="F51" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="G51" s="116"/>
+      <c r="G51" s="93"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="142"/>
-      <c r="B52" s="140" t="s">
+      <c r="A52" s="155"/>
+      <c r="B52" s="111" t="s">
         <v>117</v>
       </c>
-      <c r="C52" s="140" t="s">
+      <c r="C52" s="111" t="s">
         <v>118</v>
       </c>
-      <c r="D52" s="140" t="s">
+      <c r="D52" s="111" t="s">
         <v>116</v>
       </c>
-      <c r="E52" s="141" t="s">
+      <c r="E52" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="F52" s="140"/>
-      <c r="G52" s="143"/>
+      <c r="F52" s="111"/>
+      <c r="G52" s="113"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="117"/>
-      <c r="B53" s="118"/>
-      <c r="C53" s="118" t="s">
+      <c r="A53" s="156"/>
+      <c r="B53" s="94"/>
+      <c r="C53" s="94" t="s">
         <v>141</v>
       </c>
-      <c r="D53" s="118" t="s">
+      <c r="D53" s="94" t="s">
         <v>142</v>
       </c>
-      <c r="E53" s="119" t="s">
+      <c r="E53" s="95" t="s">
         <v>89</v>
       </c>
-      <c r="F53" s="118"/>
-      <c r="G53" s="144"/>
+      <c r="F53" s="94"/>
+      <c r="G53" s="114"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="120" t="s">
+      <c r="A55" s="132" t="s">
         <v>119</v>
       </c>
-      <c r="B55" s="121"/>
-      <c r="C55" s="121"/>
-      <c r="D55" s="121" t="s">
+      <c r="B55" s="96"/>
+      <c r="C55" s="96"/>
+      <c r="D55" s="96" t="s">
         <v>120</v>
       </c>
-      <c r="E55" s="122" t="s">
+      <c r="E55" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="F55" s="121"/>
-      <c r="G55" s="123"/>
+      <c r="F55" s="96"/>
+      <c r="G55" s="98"/>
     </row>
     <row r="56" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="124"/>
-      <c r="B56" s="125" t="s">
+      <c r="A56" s="133"/>
+      <c r="B56" s="99" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="125" t="s">
+      <c r="C56" s="99" t="s">
         <v>126</v>
       </c>
-      <c r="D56" s="125" t="s">
+      <c r="D56" s="99" t="s">
         <v>121</v>
       </c>
-      <c r="E56" s="126" t="s">
+      <c r="E56" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="F56" s="125"/>
-      <c r="G56" s="127"/>
+      <c r="F56" s="99"/>
+      <c r="G56" s="101"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="128" t="s">
+      <c r="A58" s="134" t="s">
         <v>123</v>
       </c>
-      <c r="B58" s="129"/>
-      <c r="C58" s="129"/>
-      <c r="D58" s="129" t="s">
+      <c r="B58" s="102"/>
+      <c r="C58" s="102"/>
+      <c r="D58" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="E58" s="130" t="s">
+      <c r="E58" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="F58" s="129" t="s">
+      <c r="F58" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="G58" s="131"/>
+      <c r="G58" s="104"/>
     </row>
     <row r="59" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="132"/>
-      <c r="B59" s="133" t="s">
+      <c r="A59" s="135"/>
+      <c r="B59" s="105" t="s">
         <v>129</v>
       </c>
-      <c r="C59" s="133" t="s">
+      <c r="C59" s="105" t="s">
         <v>128</v>
       </c>
-      <c r="D59" s="133" t="s">
+      <c r="D59" s="105" t="s">
         <v>125</v>
       </c>
-      <c r="E59" s="134" t="s">
+      <c r="E59" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="F59" s="133" t="s">
+      <c r="F59" s="105" t="s">
         <v>127</v>
       </c>
-      <c r="G59" s="135"/>
+      <c r="G59" s="107"/>
     </row>
     <row r="60" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="150" t="s">
+      <c r="A61" s="136" t="s">
         <v>131</v>
       </c>
-      <c r="B61" s="151" t="s">
+      <c r="B61" s="120" t="s">
         <v>129</v>
       </c>
-      <c r="C61" s="151" t="s">
+      <c r="C61" s="120" t="s">
         <v>132</v>
       </c>
-      <c r="D61" s="151" t="s">
+      <c r="D61" s="120" t="s">
         <v>133</v>
       </c>
-      <c r="E61" s="152" t="s">
+      <c r="E61" s="121" t="s">
         <v>89</v>
       </c>
-      <c r="F61" s="151" t="s">
+      <c r="F61" s="120" t="s">
         <v>134</v>
       </c>
-      <c r="G61" s="153"/>
+      <c r="G61" s="122"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="154"/>
-      <c r="B62" s="147" t="s">
+      <c r="A62" s="137"/>
+      <c r="B62" s="117" t="s">
         <v>122</v>
       </c>
-      <c r="C62" s="148" t="s">
+      <c r="C62" s="118" t="s">
         <v>136</v>
       </c>
-      <c r="D62" s="148" t="s">
+      <c r="D62" s="118" t="s">
         <v>138</v>
       </c>
-      <c r="E62" s="149" t="s">
+      <c r="E62" s="119" t="s">
         <v>135</v>
       </c>
-      <c r="F62" s="148" t="s">
+      <c r="F62" s="118" t="s">
         <v>140</v>
       </c>
-      <c r="G62" s="155"/>
+      <c r="G62" s="123"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="154"/>
-      <c r="B63" s="145"/>
-      <c r="C63" s="145" t="s">
+      <c r="A63" s="137"/>
+      <c r="B63" s="115"/>
+      <c r="C63" s="115" t="s">
         <v>137</v>
       </c>
-      <c r="D63" s="145" t="s">
+      <c r="D63" s="115" t="s">
         <v>139</v>
       </c>
-      <c r="E63" s="146" t="s">
+      <c r="E63" s="116" t="s">
         <v>89</v>
       </c>
-      <c r="F63" s="145" t="s">
+      <c r="F63" s="115" t="s">
         <v>78</v>
       </c>
-      <c r="G63" s="156"/>
+      <c r="G63" s="124"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="154"/>
-      <c r="B64" s="148" t="s">
+      <c r="A64" s="137"/>
+      <c r="B64" s="118" t="s">
         <v>143</v>
       </c>
-      <c r="C64" s="148" t="s">
+      <c r="C64" s="118" t="s">
         <v>144</v>
       </c>
-      <c r="D64" s="148" t="s">
+      <c r="D64" s="118" t="s">
         <v>145</v>
       </c>
-      <c r="E64" s="149" t="s">
+      <c r="E64" s="119" t="s">
         <v>6</v>
       </c>
-      <c r="F64" s="148" t="s">
+      <c r="F64" s="118" t="s">
         <v>146</v>
       </c>
-      <c r="G64" s="155"/>
+      <c r="G64" s="123"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="154"/>
-      <c r="B65" s="145" t="s">
+      <c r="A65" s="137"/>
+      <c r="B65" s="115" t="s">
         <v>147</v>
       </c>
-      <c r="C65" s="145" t="s">
+      <c r="C65" s="115" t="s">
         <v>148</v>
       </c>
-      <c r="D65" s="145" t="s">
+      <c r="D65" s="115" t="s">
         <v>150</v>
       </c>
-      <c r="E65" s="146" t="s">
+      <c r="E65" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="F65" s="145" t="s">
+      <c r="F65" s="115" t="s">
         <v>78</v>
       </c>
-      <c r="G65" s="156"/>
+      <c r="G65" s="124"/>
     </row>
     <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="157"/>
-      <c r="B66" s="158"/>
-      <c r="C66" s="158" t="s">
+      <c r="A66" s="138"/>
+      <c r="B66" s="125"/>
+      <c r="C66" s="125" t="s">
         <v>149</v>
       </c>
-      <c r="D66" s="158" t="s">
+      <c r="D66" s="125" t="s">
         <v>151</v>
       </c>
-      <c r="E66" s="159" t="s">
+      <c r="E66" s="126" t="s">
         <v>89</v>
       </c>
-      <c r="F66" s="158" t="s">
+      <c r="F66" s="125" t="s">
         <v>78</v>
       </c>
-      <c r="G66" s="160"/>
+      <c r="G66" s="127"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F68" s="161" t="s">
+      <c r="F68" s="128" t="s">
         <v>152</v>
       </c>
       <c r="G68" s="7">
@@ -2891,6 +2891,9 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A15:A21"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="A58:A59"/>
     <mergeCell ref="A61:A66"/>
@@ -2900,9 +2903,6 @@
     <mergeCell ref="A41:A43"/>
     <mergeCell ref="A45:A49"/>
     <mergeCell ref="A51:A53"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A15:A21"/>
   </mergeCells>
   <conditionalFormatting sqref="G54:G1048576 G1:G52">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">

</xml_diff>